<commit_message>
delete unused __pycache__ directory
</commit_message>
<xml_diff>
--- a/data/搜索指标DIFF报告示范.xlsx
+++ b/data/搜索指标DIFF报告示范.xlsx
@@ -665,7 +665,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -710,6 +710,9 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1112,27 +1115,27 @@
   </cols>
   <sheetData>
     <row r="1" ht="17.4" customHeight="1" s="13">
-      <c r="A1" s="18" t="inlineStr">
+      <c r="A1" s="19" t="inlineStr">
         <is>
           <t>字段路径</t>
         </is>
       </c>
-      <c r="B1" s="18" t="inlineStr">
+      <c r="B1" s="19" t="inlineStr">
         <is>
           <t>相似度</t>
         </is>
       </c>
-      <c r="C1" s="18" t="inlineStr">
+      <c r="C1" s="19" t="inlineStr">
         <is>
           <t>请求占比</t>
         </is>
       </c>
-      <c r="D1" s="18" t="inlineStr">
+      <c r="D1" s="19" t="inlineStr">
         <is>
           <t>数量</t>
         </is>
       </c>
-      <c r="E1" s="18" t="inlineStr">
+      <c r="E1" s="19" t="inlineStr">
         <is>
           <t>请求总数</t>
         </is>

</xml_diff>